<commit_message>
added the max and min val extraction of faster velocities
</commit_message>
<xml_diff>
--- a/data/Max_vel_EMA.xlsx
+++ b/data/Max_vel_EMA.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,50 +463,50 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.9202335569232825</v>
+        <v>3.224527022069985</v>
       </c>
       <c r="C2" t="n">
-        <v>0.07340375763576994</v>
+        <v>0.4303076923076861</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3392343568706712</v>
+        <v>2.200247722890435</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.8492396691774646</v>
+        <v>5.017727724301893</v>
       </c>
       <c r="C3" t="n">
-        <v>0.002093405257346089</v>
+        <v>1.192075471698175</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1452038492516329</v>
+        <v>2.56758812304397</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>0.9622641509434152</v>
+        <v>6.058208123693171</v>
       </c>
       <c r="C4" t="n">
-        <v>0.003085627635665976</v>
+        <v>0.03011060752624568</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1799304871007972</v>
+        <v>2.780359632897774</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
@@ -514,33 +514,33 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.5166787557690354</v>
+        <v>6.502307153373422</v>
       </c>
       <c r="C5" t="n">
-        <v>0.001941214851837425</v>
+        <v>0.4055465384618164</v>
       </c>
       <c r="D5" t="n">
-        <v>0.09479348883139295</v>
+        <v>2.616139552332734</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>1.096153846153378</v>
+        <v>6.506662497959499</v>
       </c>
       <c r="C6" t="n">
-        <v>0.02467553896589154</v>
+        <v>0.9346153846149996</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3516198277091507</v>
+        <v>3.557341617514473</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7">
@@ -548,67 +548,67 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.033676514390922</v>
+        <v>6.832291185558966</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0374183493237762</v>
+        <v>0.8019002977172413</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3499127278810166</v>
+        <v>3.574165117909011</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>1.308039315429898</v>
+        <v>7.007303065176954</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1261644528767285</v>
+        <v>1.208349552046817</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6237375423548637</v>
+        <v>3.670368983392674</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B9" t="n">
-        <v>2.644216375950668</v>
+        <v>7.140300006252018</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1167248529677674</v>
+        <v>0.03269230769228667</v>
       </c>
       <c r="D9" t="n">
-        <v>0.7116771102464662</v>
+        <v>2.87181676555667</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B10" t="n">
-        <v>3.380439387995255</v>
+        <v>7.204175618574698</v>
       </c>
       <c r="C10" t="n">
-        <v>0.01334615384616432</v>
+        <v>0.9628301886772278</v>
       </c>
       <c r="D10" t="n">
-        <v>1.028005978219535</v>
+        <v>4.239491019845341</v>
       </c>
       <c r="E10" t="n">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11">
@@ -616,33 +616,33 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>2.8313158826626</v>
+        <v>7.319653227228007</v>
       </c>
       <c r="C11" t="n">
-        <v>0.3064610312337053</v>
+        <v>0.8665471698132209</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9364851344535454</v>
+        <v>4.107759778399636</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" t="n">
-        <v>3.244335577545552</v>
+        <v>7.449228334285237</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2513587542386637</v>
+        <v>2.024999999994753</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9488329827987666</v>
+        <v>3.973527697547891</v>
       </c>
       <c r="E12" t="n">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13">
@@ -650,16 +650,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>3.666881918757972</v>
+        <v>8.042978795385023</v>
       </c>
       <c r="C13" t="n">
-        <v>0.1465180044547355</v>
+        <v>1.173076923079015</v>
       </c>
       <c r="D13" t="n">
-        <v>1.033953449776425</v>
+        <v>4.729913846844585</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14">
@@ -667,16 +667,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>3.823274501825924</v>
+        <v>9.943035929477109</v>
       </c>
       <c r="C14" t="n">
-        <v>0.09644449163348209</v>
+        <v>0.9016981132095278</v>
       </c>
       <c r="D14" t="n">
-        <v>1.43056115783137</v>
+        <v>4.231798067810463</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15">
@@ -684,67 +684,67 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>3.769230769221007</v>
+        <v>10.73008926814916</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0482905549706046</v>
+        <v>1.134615384617412</v>
       </c>
       <c r="D15" t="n">
-        <v>1.638589639294016</v>
+        <v>5.674282665135046</v>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B16" t="n">
-        <v>3.9563954402793</v>
+        <v>13.61812641318192</v>
       </c>
       <c r="C16" t="n">
-        <v>0.08873547807712637</v>
+        <v>1.150943396228942</v>
       </c>
       <c r="D16" t="n">
-        <v>1.614096567288316</v>
+        <v>6.932493868182127</v>
       </c>
       <c r="E16" t="n">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="n">
-        <v>4.158962754233138</v>
+        <v>13.94370381924824</v>
       </c>
       <c r="C17" t="n">
-        <v>0.5392817853831522</v>
+        <v>1.497532199852669</v>
       </c>
       <c r="D17" t="n">
-        <v>1.657196290762778</v>
+        <v>4.880754721054931</v>
       </c>
       <c r="E17" t="n">
-        <v>16</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" t="n">
-        <v>4.339959912477621</v>
+        <v>14.1730803056007</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6974011791596244</v>
+        <v>1.267452830186021</v>
       </c>
       <c r="D18" t="n">
-        <v>1.846624165725166</v>
+        <v>6.462416294611288</v>
       </c>
       <c r="E18" t="n">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19">
@@ -752,16 +752,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>4.945713598005694</v>
+        <v>18.15538701177616</v>
       </c>
       <c r="C19" t="n">
-        <v>0.451447269229591</v>
+        <v>0.9169811320774854</v>
       </c>
       <c r="D19" t="n">
-        <v>1.931959738982253</v>
+        <v>6.967957590559131</v>
       </c>
       <c r="E19" t="n">
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20">
@@ -769,16 +769,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>6.104391822317587</v>
+        <v>22.08100944545769</v>
       </c>
       <c r="C20" t="n">
-        <v>0.262492327856676</v>
+        <v>0.7318038461519545</v>
       </c>
       <c r="D20" t="n">
-        <v>2.45798938688743</v>
+        <v>7.527090193302703</v>
       </c>
       <c r="E20" t="n">
-        <v>19</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21">
@@ -786,16 +786,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>5.147062268336473</v>
+        <v>22.89976292736893</v>
       </c>
       <c r="C21" t="n">
-        <v>1.496778594226899</v>
+        <v>1.574150943399682</v>
       </c>
       <c r="D21" t="n">
-        <v>2.904751978913275</v>
+        <v>8.331171677261674</v>
       </c>
       <c r="E21" t="n">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22">
@@ -803,16 +803,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>7.616632873577684</v>
+        <v>26.71644666767391</v>
       </c>
       <c r="C22" t="n">
-        <v>0.8373574402420668</v>
+        <v>1.037423076920388</v>
       </c>
       <c r="D22" t="n">
-        <v>3.537650614646082</v>
+        <v>10.60695652834807</v>
       </c>
       <c r="E22" t="n">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23">
@@ -820,16 +820,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>8.142332932752149</v>
+        <v>29.28445082941915</v>
       </c>
       <c r="C23" t="n">
-        <v>0.319049971655774</v>
+        <v>0.9509433962284997</v>
       </c>
       <c r="D23" t="n">
-        <v>3.949689834618659</v>
+        <v>11.46025464117985</v>
       </c>
       <c r="E23" t="n">
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24">
@@ -837,16 +837,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>14.37118625011083</v>
+        <v>32.03906722095201</v>
       </c>
       <c r="C24" t="n">
-        <v>1.282293710222895</v>
+        <v>1.940943396214029</v>
       </c>
       <c r="D24" t="n">
-        <v>5.405177083303963</v>
+        <v>12.05980280035349</v>
       </c>
       <c r="E24" t="n">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25">
@@ -854,16 +854,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>17.53435709833348</v>
+        <v>35.35890260333666</v>
       </c>
       <c r="C25" t="n">
-        <v>0.8431961698131554</v>
+        <v>1.488461538457684</v>
       </c>
       <c r="D25" t="n">
-        <v>6.431531611494826</v>
+        <v>12.93863378955715</v>
       </c>
       <c r="E25" t="n">
-        <v>24</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26">
@@ -871,16 +871,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>18.80223072824799</v>
+        <v>39.69305188421033</v>
       </c>
       <c r="C26" t="n">
-        <v>0.9346153846129392</v>
+        <v>1.103773584908093</v>
       </c>
       <c r="D26" t="n">
-        <v>7.35722443416926</v>
+        <v>14.25693622526506</v>
       </c>
       <c r="E26" t="n">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27">
@@ -888,16 +888,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>24.91975468552197</v>
+        <v>43.4299232595142</v>
       </c>
       <c r="C27" t="n">
-        <v>1.280215125007865</v>
+        <v>1.177615384622636</v>
       </c>
       <c r="D27" t="n">
-        <v>9.621503653526281</v>
+        <v>16.08602032904356</v>
       </c>
       <c r="E27" t="n">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28">
@@ -905,16 +905,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>28.54897552595371</v>
+        <v>46.94285669597549</v>
       </c>
       <c r="C28" t="n">
-        <v>0.3459634615375747</v>
+        <v>0.7448076923057587</v>
       </c>
       <c r="D28" t="n">
-        <v>10.41987544335883</v>
+        <v>18.11461769960371</v>
       </c>
       <c r="E28" t="n">
-        <v>27</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29">
@@ -922,16 +922,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>29.23886036235944</v>
+        <v>54.40747718838475</v>
       </c>
       <c r="C29" t="n">
-        <v>1.562264150946823</v>
+        <v>2.111111111107696</v>
       </c>
       <c r="D29" t="n">
-        <v>12.10059297548423</v>
+        <v>19.10899817243011</v>
       </c>
       <c r="E29" t="n">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30">
@@ -939,16 +939,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>36.96946380078818</v>
+        <v>56.46907761695062</v>
       </c>
       <c r="C30" t="n">
-        <v>1.314814814812684</v>
+        <v>1.301886792455689</v>
       </c>
       <c r="D30" t="n">
-        <v>14.49968070098351</v>
+        <v>20.15792708430115</v>
       </c>
       <c r="E30" t="n">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31">
@@ -956,16 +956,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>38.75162807723638</v>
+        <v>64.02451668980562</v>
       </c>
       <c r="C31" t="n">
-        <v>1.423076923073236</v>
+        <v>1.426415094330519</v>
       </c>
       <c r="D31" t="n">
-        <v>16.72186913617701</v>
+        <v>22.57665739693843</v>
       </c>
       <c r="E31" t="n">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32">
@@ -973,16 +973,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>41.83572206019014</v>
+        <v>68.88583006453099</v>
       </c>
       <c r="C32" t="n">
-        <v>2.370370370366532</v>
+        <v>0.8691923076900591</v>
       </c>
       <c r="D32" t="n">
-        <v>18.14926381723847</v>
+        <v>23.96935159711744</v>
       </c>
       <c r="E32" t="n">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33">
@@ -990,16 +990,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>44.92675190909526</v>
+        <v>74.1946375362315</v>
       </c>
       <c r="C33" t="n">
-        <v>1.103019230766373</v>
+        <v>1.499999999997574</v>
       </c>
       <c r="D33" t="n">
-        <v>19.45332052923916</v>
+        <v>26.27261560040765</v>
       </c>
       <c r="E33" t="n">
-        <v>32</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34">
@@ -1007,16 +1007,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>47.21386516845421</v>
+        <v>80.35591839345615</v>
       </c>
       <c r="C34" t="n">
-        <v>1.079999999998255</v>
+        <v>2.301886792457884</v>
       </c>
       <c r="D34" t="n">
-        <v>21.49073777282373</v>
+        <v>29.93280605230369</v>
       </c>
       <c r="E34" t="n">
-        <v>33</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35">
@@ -1024,16 +1024,67 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>51.94981551080665</v>
+        <v>86.31623225422385</v>
       </c>
       <c r="C35" t="n">
-        <v>1.076923076929708</v>
+        <v>1.692307692318113</v>
       </c>
       <c r="D35" t="n">
-        <v>25.1089111729558</v>
+        <v>30.59475921304521</v>
       </c>
       <c r="E35" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
         <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>88.91008838885136</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1.519230769240122</v>
+      </c>
+      <c r="D36" t="n">
+        <v>34.39841335529584</v>
+      </c>
+      <c r="E36" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>95.37638916184267</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1.867924528305994</v>
+      </c>
+      <c r="D37" t="n">
+        <v>35.15877088448077</v>
+      </c>
+      <c r="E37" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>97.95011005340551</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1.849056603777644</v>
+      </c>
+      <c r="D38" t="n">
+        <v>38.16469754826695</v>
+      </c>
+      <c r="E38" t="n">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1047,7 +1098,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1079,138 +1130,138 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1.076923076922628</v>
+        <v>3.265247481868415</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01768652659657513</v>
+        <v>0.05453325699848422</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2634853872379855</v>
+        <v>1.778523443849014</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.9811320754717411</v>
+        <v>3.60932619590064</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01330279464727134</v>
+        <v>0.2767765924528511</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2333170116949427</v>
+        <v>1.908841990308337</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>1.031780819269258</v>
+        <v>3.862554615453487</v>
       </c>
       <c r="C4" t="n">
-        <v>0.01394450004327118</v>
+        <v>0.2804813215899696</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1905913669024969</v>
+        <v>1.859042262300695</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1.037735849056652</v>
+        <v>3.93705769230611</v>
       </c>
       <c r="C5" t="n">
-        <v>0.01266323721235607</v>
+        <v>1.050913028877835</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2415064261243034</v>
+        <v>2.394963987231358</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="n">
-        <v>1.110658819006556</v>
+        <v>4.05402682202106</v>
       </c>
       <c r="C6" t="n">
-        <v>0.07040660267741539</v>
+        <v>0.4976932455620412</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4057587099332372</v>
+        <v>1.956737340614207</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="n">
-        <v>1.654868541098267</v>
+        <v>4.091673076921421</v>
       </c>
       <c r="C7" t="n">
-        <v>0.03300943806083772</v>
+        <v>0.6506954807814778</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5125624942843071</v>
+        <v>2.347876036351284</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>1.257377197882126</v>
+        <v>4.161235488609599</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1995560203382394</v>
+        <v>0.03884054971154422</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6346618830850752</v>
+        <v>2.231154486075508</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="n">
-        <v>1.491796026561103</v>
+        <v>4.220942307690597</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2384778052975418</v>
+        <v>0.6756128490566213</v>
       </c>
       <c r="D9" t="n">
-        <v>0.7238203106818534</v>
+        <v>2.505317577313615</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10">
@@ -1218,118 +1269,118 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>1.429941865316834</v>
+        <v>5.174405133256483</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2807268011534373</v>
+        <v>0.9564099622642011</v>
       </c>
       <c r="D10" t="n">
-        <v>0.7739873670892552</v>
+        <v>2.782989968592865</v>
       </c>
       <c r="E10" t="n">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>2.140520349719676</v>
+        <v>5.639408481096846</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1981928859736377</v>
+        <v>0.9881329809628853</v>
       </c>
       <c r="D11" t="n">
-        <v>0.8372217512312005</v>
+        <v>3.359746196353791</v>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="n">
-        <v>1.801850689817281</v>
+        <v>5.656552577015648</v>
       </c>
       <c r="C12" t="n">
-        <v>0.02801328064335246</v>
+        <v>0.7604594674163349</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9332217977429568</v>
+        <v>2.793449256411428</v>
       </c>
       <c r="E12" t="n">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>3.033807849992467</v>
+        <v>7.7768306591471</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2647384543185549</v>
+        <v>0.5854920641606404</v>
       </c>
       <c r="D13" t="n">
-        <v>1.079692310737288</v>
+        <v>3.500307015450605</v>
       </c>
       <c r="E13" t="n">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="n">
-        <v>2.925689982158767</v>
+        <v>7.811223684284456</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1193396226417783</v>
+        <v>0.3385384615375929</v>
       </c>
       <c r="D14" t="n">
-        <v>1.163258061886653</v>
+        <v>3.255325081039185</v>
       </c>
       <c r="E14" t="n">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>1.965245494049669</v>
+        <v>8.123425089045559</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1701538461533794</v>
+        <v>0.8087987997346893</v>
       </c>
       <c r="D15" t="n">
-        <v>1.147098710863492</v>
+        <v>4.369685846404618</v>
       </c>
       <c r="E15" t="n">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="n">
-        <v>3.589105065181662</v>
+        <v>8.60107175512767</v>
       </c>
       <c r="C16" t="n">
-        <v>0.2637785293532227</v>
+        <v>0.3500000000006285</v>
       </c>
       <c r="D16" t="n">
-        <v>1.301100035748837</v>
+        <v>4.175228328467653</v>
       </c>
       <c r="E16" t="n">
-        <v>16</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17">
@@ -1337,16 +1388,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>3.5380752679839</v>
+        <v>10.44812841525584</v>
       </c>
       <c r="C17" t="n">
-        <v>0.3818091383507187</v>
+        <v>0.6519807692319071</v>
       </c>
       <c r="D17" t="n">
-        <v>1.710851738366202</v>
+        <v>4.825161143986494</v>
       </c>
       <c r="E17" t="n">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18">
@@ -1354,16 +1405,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>3.705913167957617</v>
+        <v>11.15674758095643</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1403773014008918</v>
+        <v>0.9344423076939757</v>
       </c>
       <c r="D18" t="n">
-        <v>1.841848537878289</v>
+        <v>5.367744843052963</v>
       </c>
       <c r="E18" t="n">
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19">
@@ -1371,16 +1422,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>4.455271468326681</v>
+        <v>15.37757077598665</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1830540374306301</v>
+        <v>1.630188679248852</v>
       </c>
       <c r="D19" t="n">
-        <v>2.095850410941058</v>
+        <v>6.292929917653573</v>
       </c>
       <c r="E19" t="n">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20">
@@ -1388,16 +1439,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>3.973002342646011</v>
+        <v>16.37724893603309</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1885378930956361</v>
+        <v>1.773584905664262</v>
       </c>
       <c r="D20" t="n">
-        <v>2.399443331490241</v>
+        <v>7.083391424737282</v>
       </c>
       <c r="E20" t="n">
-        <v>20</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21">
@@ -1405,16 +1456,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>5.134527304511706</v>
+        <v>19.04316832414464</v>
       </c>
       <c r="C21" t="n">
-        <v>0.6189862928824361</v>
+        <v>1.207358490568665</v>
       </c>
       <c r="D21" t="n">
-        <v>2.774505870218417</v>
+        <v>7.677261472364897</v>
       </c>
       <c r="E21" t="n">
-        <v>21</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22">
@@ -1422,16 +1473,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>7.914876578688168</v>
+        <v>21.11449646189762</v>
       </c>
       <c r="C22" t="n">
-        <v>1.001664084805094</v>
+        <v>1.01923076923706</v>
       </c>
       <c r="D22" t="n">
-        <v>3.331821694406732</v>
+        <v>8.804544733408832</v>
       </c>
       <c r="E22" t="n">
-        <v>22</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23">
@@ -1439,16 +1490,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>7.408188618448484</v>
+        <v>22.60462203395683</v>
       </c>
       <c r="C23" t="n">
-        <v>0.5629186592293003</v>
+        <v>1.137735849049337</v>
       </c>
       <c r="D23" t="n">
-        <v>3.828047393582893</v>
+        <v>9.096650239828747</v>
       </c>
       <c r="E23" t="n">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24">
@@ -1456,16 +1507,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>10.02222583577328</v>
+        <v>26.89770447459302</v>
       </c>
       <c r="C24" t="n">
-        <v>1.018867924530545</v>
+        <v>0.3396980769251655</v>
       </c>
       <c r="D24" t="n">
-        <v>4.48860685857232</v>
+        <v>9.798789656986255</v>
       </c>
       <c r="E24" t="n">
-        <v>24</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25">
@@ -1473,16 +1524,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>12.64900398271503</v>
+        <v>30.41361244723486</v>
       </c>
       <c r="C25" t="n">
-        <v>0.8999999999985526</v>
+        <v>1.324528301889698</v>
       </c>
       <c r="D25" t="n">
-        <v>5.503417075064901</v>
+        <v>11.85251219381296</v>
       </c>
       <c r="E25" t="n">
-        <v>25</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26">
@@ -1490,16 +1541,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>14.74190154627803</v>
+        <v>33.21496780414908</v>
       </c>
       <c r="C26" t="n">
-        <v>0.6018455769215266</v>
+        <v>1.918867924532502</v>
       </c>
       <c r="D26" t="n">
-        <v>6.417948256949881</v>
+        <v>12.39912147854833</v>
       </c>
       <c r="E26" t="n">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27">
@@ -1507,16 +1558,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>18.7359584578763</v>
+        <v>36.93384868527497</v>
       </c>
       <c r="C27" t="n">
-        <v>1.283333333331261</v>
+        <v>2.5740740740699</v>
       </c>
       <c r="D27" t="n">
-        <v>7.862491370067854</v>
+        <v>14.27051750029366</v>
       </c>
       <c r="E27" t="n">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28">
@@ -1524,16 +1575,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>22.44895050095267</v>
+        <v>40.23810528156042</v>
       </c>
       <c r="C28" t="n">
-        <v>1.137115384612435</v>
+        <v>1.115384615381725</v>
       </c>
       <c r="D28" t="n">
-        <v>9.051658820761139</v>
+        <v>14.9569904992655</v>
       </c>
       <c r="E28" t="n">
-        <v>28</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29">
@@ -1541,16 +1592,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>23.9687310413997</v>
+        <v>43.15042562766019</v>
       </c>
       <c r="C29" t="n">
-        <v>0.9300217499975937</v>
+        <v>1.409433962255153</v>
       </c>
       <c r="D29" t="n">
-        <v>10.64802769390724</v>
+        <v>15.89478281624042</v>
       </c>
       <c r="E29" t="n">
-        <v>29</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30">
@@ -1558,16 +1609,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>26.46633954574956</v>
+        <v>43.59827366805098</v>
       </c>
       <c r="C30" t="n">
-        <v>1.236496153853772</v>
+        <v>0.9346153846211467</v>
       </c>
       <c r="D30" t="n">
-        <v>11.70531363311794</v>
+        <v>16.86511812634048</v>
       </c>
       <c r="E30" t="n">
-        <v>30</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31">
@@ -1575,16 +1626,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>30.86215264787391</v>
+        <v>50.18988359638066</v>
       </c>
       <c r="C31" t="n">
-        <v>1.261730769238528</v>
+        <v>0.969230769228256</v>
       </c>
       <c r="D31" t="n">
-        <v>12.91676610282385</v>
+        <v>18.23496978982583</v>
       </c>
       <c r="E31" t="n">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32">
@@ -1592,16 +1643,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>30.5032416919706</v>
+        <v>51.71012091177425</v>
       </c>
       <c r="C32" t="n">
-        <v>0.9533076923135519</v>
+        <v>1.249999999996755</v>
       </c>
       <c r="D32" t="n">
-        <v>13.80078029031775</v>
+        <v>20.17951510264986</v>
       </c>
       <c r="E32" t="n">
-        <v>32</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33">
@@ -1609,16 +1660,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>35.31036053317028</v>
+        <v>55.59006644799854</v>
       </c>
       <c r="C33" t="n">
-        <v>1.199423076930453</v>
+        <v>1.980769230764099</v>
       </c>
       <c r="D33" t="n">
-        <v>16.31776266320879</v>
+        <v>22.85818844259163</v>
       </c>
       <c r="E33" t="n">
-        <v>33</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34">
@@ -1626,16 +1677,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>38.2949440696739</v>
+        <v>58.96202106914039</v>
       </c>
       <c r="C34" t="n">
-        <v>1.451886792456021</v>
+        <v>1.033333333331656</v>
       </c>
       <c r="D34" t="n">
-        <v>17.82709011689602</v>
+        <v>22.33650912106451</v>
       </c>
       <c r="E34" t="n">
-        <v>34</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35">
@@ -1643,16 +1694,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>40.06013612925789</v>
+        <v>62.79234936069401</v>
       </c>
       <c r="C35" t="n">
-        <v>0.7620663396112268</v>
+        <v>1.096153846160602</v>
       </c>
       <c r="D35" t="n">
-        <v>18.38605110161502</v>
+        <v>23.85989181007575</v>
       </c>
       <c r="E35" t="n">
-        <v>35</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36">
@@ -1660,16 +1711,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>41.1391877012449</v>
+        <v>65.77786924725898</v>
       </c>
       <c r="C36" t="n">
-        <v>2.215384615398249</v>
+        <v>2.65384615386249</v>
       </c>
       <c r="D36" t="n">
-        <v>20.12010740332173</v>
+        <v>26.43952856861182</v>
       </c>
       <c r="E36" t="n">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37">
@@ -1677,50 +1728,50 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>44.58897783558025</v>
+        <v>68.39269895092363</v>
       </c>
       <c r="C37" t="n">
-        <v>1.834615384626674</v>
+        <v>0.8131153846203936</v>
       </c>
       <c r="D37" t="n">
-        <v>22.67324751865245</v>
+        <v>27.1555734809889</v>
       </c>
       <c r="E37" t="n">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>46.21461579327901</v>
+        <v>72.66130658263312</v>
       </c>
       <c r="C38" t="n">
-        <v>0.7798924528319172</v>
+        <v>2.277777777812446</v>
       </c>
       <c r="D38" t="n">
-        <v>23.38013147150151</v>
+        <v>33.18674070518679</v>
       </c>
       <c r="E38" t="n">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" t="n">
-        <v>49.43633647145184</v>
+        <v>72.81214506540614</v>
       </c>
       <c r="C39" t="n">
-        <v>2.269230769205023</v>
+        <v>1.29807692308493</v>
       </c>
       <c r="D39" t="n">
-        <v>25.38824157989664</v>
+        <v>30.00396195686887</v>
       </c>
       <c r="E39" t="n">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40">
@@ -1728,16 +1779,84 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>51.21602823457858</v>
+        <v>77.73052058117538</v>
       </c>
       <c r="C40" t="n">
-        <v>1.247711538447392</v>
+        <v>0.9807692307752378</v>
       </c>
       <c r="D40" t="n">
-        <v>27.09888834359075</v>
+        <v>33.18511495099995</v>
       </c>
       <c r="E40" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>82.30992737394087</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1.409433962267246</v>
+      </c>
+      <c r="D41" t="n">
+        <v>35.53660569400386</v>
+      </c>
+      <c r="E41" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>87.0683839566986</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1.349999999997829</v>
+      </c>
+      <c r="D42" t="n">
+        <v>37.83902452460546</v>
+      </c>
+      <c r="E42" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>89.49149721411602</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1.807692307671826</v>
+      </c>
+      <c r="D43" t="n">
+        <v>40.37313595807398</v>
+      </c>
+      <c r="E43" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>94.06828494812044</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1.711538461549007</v>
+      </c>
+      <c r="D44" t="n">
+        <v>42.56928084680181</v>
+      </c>
+      <c r="E44" t="n">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1751,7 +1870,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1783,121 +1902,121 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.8412460588206261</v>
+        <v>-3.477503872202479</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.002304111922659488</v>
+        <v>-0.8380415769232188</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.1462554701662002</v>
+        <v>-2.032606393268657</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>-1.150943396226507</v>
+        <v>-3.527184424711415</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.6234211730773639</v>
+        <v>-0.7948903846150465</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.8662004521564172</v>
+        <v>-2.091562739833449</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.052295847347412</v>
+        <v>-3.841700966045766</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.05403256628229269</v>
+        <v>-1.018321173509493</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.4050259763574371</v>
+        <v>-2.333663247630872</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B5" t="n">
-        <v>-1.058347183444067</v>
+        <v>-3.966987001700972</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.02209516109212622</v>
+        <v>-0.87892641509433</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.3037751879277399</v>
+        <v>-2.081485627887677</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.130165498325622</v>
+        <v>-4.214680588654796</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.01642320326823369</v>
+        <v>-1.096153846153413</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.3426252629418078</v>
+        <v>-2.53741097089497</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.134615384617395</v>
+        <v>-4.652252690226288</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.03440162469009539</v>
+        <v>-0.7798924528302443</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.4153882360381311</v>
+        <v>-2.620953146928581</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" t="n">
-        <v>-1.217251114201226</v>
+        <v>-4.706744040558433</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.09885584825762546</v>
+        <v>-0.725621365385101</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.5128854495412869</v>
+        <v>-2.517638955702649</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9">
@@ -1905,16 +2024,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.211771921016943</v>
+        <v>-4.867602625838313</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.1351406828611024</v>
+        <v>-1.488461538460955</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.5180308433121229</v>
+        <v>-3.135210137097372</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10">
@@ -1922,50 +2041,50 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-1.323442384181975</v>
+        <v>-5.29391962945293</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.1475945303089601</v>
+        <v>-1.237924528301975</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.6188146897287449</v>
+        <v>-3.26331735549821</v>
       </c>
       <c r="E10" t="n">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>-1.438988420347245</v>
+        <v>-6.263596948830756</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.2666474594415889</v>
+        <v>-0.8826923076900153</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.7796672091040678</v>
+        <v>-3.584147161175249</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="n">
-        <v>-1.76893177114319</v>
+        <v>-6.315480839712197</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.2950079656179594</v>
+        <v>-1.105961538458687</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.8975394777385897</v>
+        <v>-3.387404537835098</v>
       </c>
       <c r="E12" t="n">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13">
@@ -1973,16 +2092,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>-2.188725052948453</v>
+        <v>-7.448688428589865</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.325060409912819</v>
+        <v>-1.596226415097846</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.9762690568925491</v>
+        <v>-4.084283426166238</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14">
@@ -1990,16 +2109,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-2.073658798435584</v>
+        <v>-8.716834381337881</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.4153148900098361</v>
+        <v>-0.9679245282998836</v>
       </c>
       <c r="D14" t="n">
-        <v>-1.107878158327026</v>
+        <v>-4.283317972037902</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15">
@@ -2007,16 +2126,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>-2.202374298868382</v>
+        <v>-8.969849590557242</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.579475090385644</v>
+        <v>-1.509433962267468</v>
       </c>
       <c r="D15" t="n">
-        <v>-1.28248385355816</v>
+        <v>-4.769762560288215</v>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16">
@@ -2024,16 +2143,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>-2.460349173004778</v>
+        <v>-10.41638961214733</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.4065321193388091</v>
+        <v>-2.342428301891957</v>
       </c>
       <c r="D16" t="n">
-        <v>-1.41917352525936</v>
+        <v>-5.576050279046638</v>
       </c>
       <c r="E16" t="n">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17">
@@ -2041,16 +2160,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>-2.566405735377961</v>
+        <v>-14.11264434429183</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.3712531339805445</v>
+        <v>-1.115660377360935</v>
       </c>
       <c r="D17" t="n">
-        <v>-1.441124305244996</v>
+        <v>-5.653735213617884</v>
       </c>
       <c r="E17" t="n">
-        <v>16</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18">
@@ -2058,16 +2177,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>-2.945685000858465</v>
+        <v>-15.19112213130751</v>
       </c>
       <c r="C18" t="n">
-        <v>-1.031603773587164</v>
+        <v>-1.49999999999614</v>
       </c>
       <c r="D18" t="n">
-        <v>-1.813477613221108</v>
+        <v>-6.238075686853156</v>
       </c>
       <c r="E18" t="n">
-        <v>17</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19">
@@ -2075,16 +2194,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>-3.862717182353169</v>
+        <v>-16.48099930686186</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.9668656513200583</v>
+        <v>-0.9533076923135519</v>
       </c>
       <c r="D19" t="n">
-        <v>-2.01965721117071</v>
+        <v>-6.765670004645129</v>
       </c>
       <c r="E19" t="n">
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20">
@@ -2092,16 +2211,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>-4.441630928135754</v>
+        <v>-18.96846010240972</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.6434826923060313</v>
+        <v>-0.9078113207567108</v>
       </c>
       <c r="D20" t="n">
-        <v>-2.326197942156224</v>
+        <v>-7.450818034490595</v>
       </c>
       <c r="E20" t="n">
-        <v>19</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21">
@@ -2109,16 +2228,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-6.418671896262889</v>
+        <v>-21.07468296405145</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.7477484019851475</v>
+        <v>-1.069811320757087</v>
       </c>
       <c r="D21" t="n">
-        <v>-2.766396860870936</v>
+        <v>-8.051998845862549</v>
       </c>
       <c r="E21" t="n">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22">
@@ -2126,16 +2245,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>-7.181701395457709</v>
+        <v>-22.48398551733685</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.717996226416674</v>
+        <v>-1.188679245275442</v>
       </c>
       <c r="D22" t="n">
-        <v>-3.20850489001886</v>
+        <v>-9.004366316862084</v>
       </c>
       <c r="E22" t="n">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23">
@@ -2143,16 +2262,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>-9.392932245780464</v>
+        <v>-24.80405518466924</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.762066339617799</v>
+        <v>-2.394339622626242</v>
       </c>
       <c r="D23" t="n">
-        <v>-3.782933125528829</v>
+        <v>-10.24402988000356</v>
       </c>
       <c r="E23" t="n">
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24">
@@ -2160,16 +2279,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>-11.82486886488476</v>
+        <v>-29.19405319554879</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.9755451865975491</v>
+        <v>-1.096153846151016</v>
       </c>
       <c r="D24" t="n">
-        <v>-4.635344224851058</v>
+        <v>-11.0200505401768</v>
       </c>
       <c r="E24" t="n">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25">
@@ -2177,16 +2296,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>-14.22027294154929</v>
+        <v>-31.82656415017027</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.6434826923060313</v>
+        <v>-1.370769230765678</v>
       </c>
       <c r="D25" t="n">
-        <v>-5.332174041249966</v>
+        <v>-12.12725798760935</v>
       </c>
       <c r="E25" t="n">
-        <v>24</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26">
@@ -2194,16 +2313,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>-16.47107309672464</v>
+        <v>-35.13552882094324</v>
       </c>
       <c r="C26" t="n">
-        <v>-1.142307692304738</v>
+        <v>-0.9093396226435024</v>
       </c>
       <c r="D26" t="n">
-        <v>-6.56125916017172</v>
+        <v>-12.9046227509112</v>
       </c>
       <c r="E26" t="n">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27">
@@ -2211,16 +2330,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>-16.63674511619719</v>
+        <v>-37.92653329465653</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.8289571153824769</v>
+        <v>-1.292884615392582</v>
       </c>
       <c r="D27" t="n">
-        <v>-7.407643358163415</v>
+        <v>-13.60714451714094</v>
       </c>
       <c r="E27" t="n">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28">
@@ -2228,16 +2347,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>-19.50588787063343</v>
+        <v>-41.23280923107419</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.9169811320774938</v>
+        <v>-1.490566037739135</v>
       </c>
       <c r="D28" t="n">
-        <v>-8.754632924584149</v>
+        <v>-15.50375442825021</v>
       </c>
       <c r="E28" t="n">
-        <v>27</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29">
@@ -2245,16 +2364,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>-21.69975992494612</v>
+        <v>-43.07510059454214</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.8826923076900836</v>
+        <v>-1.409433962267246</v>
       </c>
       <c r="D29" t="n">
-        <v>-9.891880356157611</v>
+        <v>-16.41010594771156</v>
       </c>
       <c r="E29" t="n">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30">
@@ -2262,16 +2381,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>-24.26574509692714</v>
+        <v>-46.23916764311696</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.6813346153828165</v>
+        <v>-1.811320754720961</v>
       </c>
       <c r="D30" t="n">
-        <v>-10.87781471097221</v>
+        <v>-17.10265553399136</v>
       </c>
       <c r="E30" t="n">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31">
@@ -2279,16 +2398,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>-27.83152849710137</v>
+        <v>-50.23438632590145</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.7788461538441672</v>
+        <v>-1.849056603777661</v>
       </c>
       <c r="D31" t="n">
-        <v>-13.02079646539988</v>
+        <v>-19.53646201798112</v>
       </c>
       <c r="E31" t="n">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32">
@@ -2296,16 +2415,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>-31.43809584356047</v>
+        <v>-54.56926735962036</v>
       </c>
       <c r="C32" t="n">
-        <v>-1.174500000007996</v>
+        <v>-1.332692307700515</v>
       </c>
       <c r="D32" t="n">
-        <v>-15.04362079970167</v>
+        <v>-21.04156559195288</v>
       </c>
       <c r="E32" t="n">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33">
@@ -2313,16 +2432,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>-33.86524316032824</v>
+        <v>-58.95465792267359</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.8490566037754821</v>
+        <v>-1.1250000000069</v>
       </c>
       <c r="D33" t="n">
-        <v>-16.54594658529733</v>
+        <v>-22.24321066952465</v>
       </c>
       <c r="E33" t="n">
-        <v>32</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34">
@@ -2330,16 +2449,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>-35.37128060229282</v>
+        <v>-59.76933209931514</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.7009615384658259</v>
+        <v>-1.980769230781421</v>
       </c>
       <c r="D34" t="n">
-        <v>-17.69134075551304</v>
+        <v>-23.62327840481401</v>
       </c>
       <c r="E34" t="n">
-        <v>33</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35">
@@ -2347,16 +2466,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>-36.43930600602259</v>
+        <v>-62.80046738829182</v>
       </c>
       <c r="C35" t="n">
-        <v>-1.980769230781455</v>
+        <v>-1.533333333330833</v>
       </c>
       <c r="D35" t="n">
-        <v>-19.14013467008744</v>
+        <v>-26.4741252956384</v>
       </c>
       <c r="E35" t="n">
-        <v>34</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36">
@@ -2364,16 +2483,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>-38.45940093902567</v>
+        <v>-64.4951043761497</v>
       </c>
       <c r="C36" t="n">
-        <v>-1.021153846142284</v>
+        <v>-1.259259259257216</v>
       </c>
       <c r="D36" t="n">
-        <v>-20.22743330041638</v>
+        <v>-26.89111812536116</v>
       </c>
       <c r="E36" t="n">
-        <v>35</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37">
@@ -2381,16 +2500,84 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>-41.16687640815498</v>
+        <v>-66.19038107133265</v>
       </c>
       <c r="C37" t="n">
-        <v>-1.043653846141997</v>
+        <v>-1.886538461517124</v>
       </c>
       <c r="D37" t="n">
-        <v>-21.38334304846926</v>
+        <v>-26.92504249729691</v>
       </c>
       <c r="E37" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
         <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>-69.99196717692602</v>
+      </c>
+      <c r="C38" t="n">
+        <v>-1.679245283022531</v>
+      </c>
+      <c r="D38" t="n">
+        <v>-29.59891848071362</v>
+      </c>
+      <c r="E38" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>-70.71120907737202</v>
+      </c>
+      <c r="C39" t="n">
+        <v>-1.409433962267246</v>
+      </c>
+      <c r="D39" t="n">
+        <v>-30.56634407357106</v>
+      </c>
+      <c r="E39" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>-71.81232801309993</v>
+      </c>
+      <c r="C40" t="n">
+        <v>-1.769230769210693</v>
+      </c>
+      <c r="D40" t="n">
+        <v>-32.31536603554112</v>
+      </c>
+      <c r="E40" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>-75.57506831531143</v>
+      </c>
+      <c r="C41" t="n">
+        <v>-1.528301886795801</v>
+      </c>
+      <c r="D41" t="n">
+        <v>-32.27837248778516</v>
+      </c>
+      <c r="E41" t="n">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2404,7 +2591,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2436,36 +2623,36 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>-1.032021917929678</v>
+        <v>-4.102900952583642</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.01368600272354659</v>
+        <v>-0.9322641509434434</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.2878451799611561</v>
+        <v>-2.689434085212524</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>-1.038461538463396</v>
+        <v>-4.5781242580184</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.0278128389443715</v>
+        <v>-0.8660377358490837</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.2874266468809935</v>
+        <v>-2.61817620892214</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
@@ -2473,16 +2660,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.104654476514315</v>
+        <v>-4.883434189955473</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.09531839109816861</v>
+        <v>-0.7570384615390061</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.4367698026276607</v>
+        <v>-3.10276526595925</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5">
@@ -2490,16 +2677,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-1.244460514427157</v>
+        <v>-5.099933686124037</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.1798688156822215</v>
+        <v>-1.023403846154554</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.5562276219444393</v>
+        <v>-3.373049846286431</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6">
@@ -2507,16 +2694,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.471408380153791</v>
+        <v>-5.525318261137103</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.238922450900442</v>
+        <v>-2.28461538461447</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.7371922693346259</v>
+        <v>-3.706783679246611</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7">
@@ -2524,16 +2711,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.623103941067569</v>
+        <v>-6.121955040378872</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.2667390066760731</v>
+        <v>-1.103773584905726</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.8155205911168982</v>
+        <v>-3.644291264912527</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -2541,16 +2728,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-1.968941720646068</v>
+        <v>-6.171178431920715</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.3611782332349123</v>
+        <v>-0.9252692307688584</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.96338377074306</v>
+        <v>-4.077682699124624</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
@@ -2558,16 +2745,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-2.183220556433114</v>
+        <v>-7.238422827472557</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.3618361170841451</v>
+        <v>-1.018867924528359</v>
       </c>
       <c r="D9" t="n">
-        <v>-1.115742591721257</v>
+        <v>-4.20185180063941</v>
       </c>
       <c r="E9" t="n">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10">
@@ -2575,16 +2762,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-2.210414734500085</v>
+        <v>-8.455234310758087</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.5234192490577414</v>
+        <v>-1.301886792450087</v>
       </c>
       <c r="D10" t="n">
-        <v>-1.276279781566332</v>
+        <v>-4.752847428231082</v>
       </c>
       <c r="E10" t="n">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
@@ -2592,16 +2779,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-2.41283186457317</v>
+        <v>-9.016160012508687</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.5702770730754608</v>
+        <v>-1.499999999997599</v>
       </c>
       <c r="D11" t="n">
-        <v>-1.521008430757798</v>
+        <v>-5.182726056941858</v>
       </c>
       <c r="E11" t="n">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12">
@@ -2609,16 +2796,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>-2.613700050597057</v>
+        <v>-10.11779613220556</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.5426830211548171</v>
+        <v>-1.711538461541523</v>
       </c>
       <c r="D12" t="n">
-        <v>-1.68422330865397</v>
+        <v>-5.657802995040555</v>
       </c>
       <c r="E12" t="n">
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13">
@@ -2626,16 +2813,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>-3.199463714183245</v>
+        <v>-11.05393475749417</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.6699790384597946</v>
+        <v>-0.9615384615359862</v>
       </c>
       <c r="D13" t="n">
-        <v>-1.908869692723064</v>
+        <v>-6.092034448352847</v>
       </c>
       <c r="E13" t="n">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14">
@@ -2643,16 +2830,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-3.183680024352534</v>
+        <v>-11.50553702352603</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.9034615384591916</v>
+        <v>-1.001886792455042</v>
       </c>
       <c r="D14" t="n">
-        <v>-2.247111357564039</v>
+        <v>-6.155845796584627</v>
       </c>
       <c r="E14" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15">
@@ -2660,16 +2847,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>-4.559870574107102</v>
+        <v>-13.70096610355787</v>
       </c>
       <c r="C15" t="n">
-        <v>-1.121538461545369</v>
+        <v>-1.443396226418252</v>
       </c>
       <c r="D15" t="n">
-        <v>-2.639171197660476</v>
+        <v>-6.844820481672793</v>
       </c>
       <c r="E15" t="n">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16">
@@ -2677,16 +2864,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>-5.432080512343926</v>
+        <v>-17.23901065564643</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.7850769230749031</v>
+        <v>-0.95094339622442</v>
       </c>
       <c r="D16" t="n">
-        <v>-3.006037088976884</v>
+        <v>-7.68445149195873</v>
       </c>
       <c r="E16" t="n">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17">
@@ -2694,16 +2881,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>-6.661816207054801</v>
+        <v>-19.48952854048428</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.7040457692289286</v>
+        <v>-1.021153846155679</v>
       </c>
       <c r="D17" t="n">
-        <v>-3.440993836902197</v>
+        <v>-8.668113593644089</v>
       </c>
       <c r="E17" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18">
@@ -2711,16 +2898,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>-8.061694591897869</v>
+        <v>-24.47129699717262</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.7641509433979339</v>
+        <v>-1.03846153845889</v>
       </c>
       <c r="D18" t="n">
-        <v>-4.091191211949869</v>
+        <v>-9.813281381994857</v>
       </c>
       <c r="E18" t="n">
-        <v>20</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19">
@@ -2728,16 +2915,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>-10.91755262007622</v>
+        <v>-27.42329534064269</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.7303754716934626</v>
+        <v>-1.203703703701781</v>
       </c>
       <c r="D19" t="n">
-        <v>-4.991500921105416</v>
+        <v>-11.47415671035305</v>
       </c>
       <c r="E19" t="n">
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20">
@@ -2745,16 +2932,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>-12.02312793064359</v>
+        <v>-29.15948846898159</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.8567307692285703</v>
+        <v>-1.615384615380427</v>
       </c>
       <c r="D20" t="n">
-        <v>-5.812329861062146</v>
+        <v>-12.22086262279521</v>
       </c>
       <c r="E20" t="n">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21">
@@ -2762,16 +2949,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-16.37642625762128</v>
+        <v>-32.20570169268718</v>
       </c>
       <c r="C21" t="n">
-        <v>-1.135557692304785</v>
+        <v>-1.094339622643977</v>
       </c>
       <c r="D21" t="n">
-        <v>-7.219023493170877</v>
+        <v>-13.6431765055779</v>
       </c>
       <c r="E21" t="n">
-        <v>23</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22">
@@ -2779,16 +2966,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>-19.37008236360059</v>
+        <v>-37.58920813706526</v>
       </c>
       <c r="C22" t="n">
-        <v>-1.443396226418252</v>
+        <v>-1.021153846151214</v>
       </c>
       <c r="D22" t="n">
-        <v>-8.917223206712753</v>
+        <v>-14.95721564355239</v>
       </c>
       <c r="E22" t="n">
-        <v>24</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23">
@@ -2796,16 +2983,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>-21.95023890425908</v>
+        <v>-40.12265301972916</v>
       </c>
       <c r="C23" t="n">
-        <v>-1.390754716984157</v>
+        <v>-1.001886792455042</v>
       </c>
       <c r="D23" t="n">
-        <v>-10.25814315506971</v>
+        <v>-16.28397420120723</v>
       </c>
       <c r="E23" t="n">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24">
@@ -2813,16 +3000,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>-25.36717607857462</v>
+        <v>-43.70212670960306</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.7430192307673337</v>
+        <v>-1.396226415097437</v>
       </c>
       <c r="D24" t="n">
-        <v>-11.83906900661307</v>
+        <v>-17.30769735850585</v>
       </c>
       <c r="E24" t="n">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25">
@@ -2830,16 +3017,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>-28.91718235134276</v>
+        <v>-47.54032920259027</v>
       </c>
       <c r="C25" t="n">
-        <v>-1.339615384611965</v>
+        <v>-1.69230769230333</v>
       </c>
       <c r="D25" t="n">
-        <v>-13.85163989075733</v>
+        <v>-18.79951013680124</v>
       </c>
       <c r="E25" t="n">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26">
@@ -2847,16 +3034,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>-32.00737184155037</v>
+        <v>-51.36344283660379</v>
       </c>
       <c r="C26" t="n">
-        <v>-1.249999999996789</v>
+        <v>-2.452830188684681</v>
       </c>
       <c r="D26" t="n">
-        <v>-15.56700009870999</v>
+        <v>-20.90993136485001</v>
       </c>
       <c r="E26" t="n">
-        <v>28</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27">
@@ -2864,16 +3051,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>-34.75540962746706</v>
+        <v>-54.82453061413113</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.1520370370367592</v>
+        <v>-1.346153846150367</v>
       </c>
       <c r="D27" t="n">
-        <v>-17.45681241338348</v>
+        <v>-22.28839447097916</v>
       </c>
       <c r="E27" t="n">
-        <v>29</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28">
@@ -2881,16 +3068,67 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>-37.59878587921698</v>
+        <v>-58.31565551363691</v>
       </c>
       <c r="C28" t="n">
-        <v>-1.730769230764816</v>
+        <v>-1.865384615379744</v>
       </c>
       <c r="D28" t="n">
-        <v>-19.24924415194241</v>
+        <v>-24.01950532890408</v>
       </c>
       <c r="E28" t="n">
-        <v>30</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>-63.16968924771424</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-1.576923076919009</v>
+      </c>
+      <c r="D29" t="n">
+        <v>-25.63939309819554</v>
+      </c>
+      <c r="E29" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>-67.90883857992162</v>
+      </c>
+      <c r="C30" t="n">
+        <v>-1.641509433965865</v>
+      </c>
+      <c r="D30" t="n">
+        <v>-28.9329347968969</v>
+      </c>
+      <c r="E30" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>-74.14174839996737</v>
+      </c>
+      <c r="C31" t="n">
+        <v>-1.273584905663223</v>
+      </c>
+      <c r="D31" t="n">
+        <v>-30.20383242566376</v>
+      </c>
+      <c r="E31" t="n">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>